<commit_message>
App update Aug 2024 at end of ZC subscription
</commit_message>
<xml_diff>
--- a/Microclimate_data_supporting/MC_bad_data_windows_Damon.xlsx
+++ b/Microclimate_data_supporting/MC_bad_data_windows_Damon.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://luky-my.sharepoint.com/personal/drva228_uky_edu/Documents/TMCF/Continuous_data/TMCF_Microclimate/Microclimate_data_supporting/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="287" documentId="8_{F172169B-6994-40F3-9A6F-FDA03E5D807A}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{AAC9ACD1-E1D5-4BC8-BDF9-9CF36F72836E}"/>
+  <xr:revisionPtr revIDLastSave="400" documentId="8_{F172169B-6994-40F3-9A6F-FDA03E5D807A}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{E66D82C8-B68E-42B1-AB11-0BE26126F012}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" xr2:uid="{2D31975C-DB24-4E04-A6AF-06E4EBFDD9C4}"/>
   </bookViews>
@@ -36,7 +36,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="133" uniqueCount="41">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="242" uniqueCount="45">
   <si>
     <t>Tree</t>
   </si>
@@ -71,9 +71,6 @@
     <t>FB3</t>
   </si>
   <si>
-    <t>Wetness</t>
-  </si>
-  <si>
     <t>S5</t>
   </si>
   <si>
@@ -159,6 +156,21 @@
   </si>
   <si>
     <t>FB4</t>
+  </si>
+  <si>
+    <t>Solar at night</t>
+  </si>
+  <si>
+    <t>Fritzing, I think the cable was chewed by the cow</t>
+  </si>
+  <si>
+    <t>LWS_Count</t>
+  </si>
+  <si>
+    <t>LW_Minutes</t>
+  </si>
+  <si>
+    <t>LW_Minutes_H</t>
   </si>
 </sst>
 </file>
@@ -535,10 +547,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{44A88BFF-DC98-4559-AC87-101535AA5E20}">
-  <dimension ref="A1:F41"/>
+  <dimension ref="A1:F76"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="E18" sqref="E18"/>
+    <sheetView tabSelected="1" topLeftCell="A49" workbookViewId="0">
+      <selection activeCell="E71" sqref="E71"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -564,18 +576,18 @@
         <v>3</v>
       </c>
       <c r="F1" t="s">
-        <v>26</v>
+        <v>25</v>
       </c>
     </row>
     <row r="2" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A2" t="s">
-        <v>33</v>
+        <v>32</v>
       </c>
       <c r="B2" t="s">
-        <v>30</v>
+        <v>29</v>
       </c>
       <c r="C2" t="s">
-        <v>23</v>
+        <v>22</v>
       </c>
       <c r="D2" s="1">
         <v>45253</v>
@@ -584,7 +596,7 @@
         <v>45316</v>
       </c>
       <c r="F2" t="s">
-        <v>34</v>
+        <v>33</v>
       </c>
     </row>
     <row r="3" spans="1:6" x14ac:dyDescent="0.25">
@@ -592,16 +604,16 @@
         <v>5</v>
       </c>
       <c r="B3" t="s">
-        <v>4</v>
+        <v>29</v>
       </c>
       <c r="C3" t="s">
         <v>7</v>
       </c>
       <c r="D3" s="1">
-        <v>45011</v>
+        <v>45090</v>
       </c>
       <c r="E3" s="1">
-        <v>45028</v>
+        <v>45134</v>
       </c>
     </row>
     <row r="4" spans="1:6" x14ac:dyDescent="0.25">
@@ -615,10 +627,10 @@
         <v>7</v>
       </c>
       <c r="D4" s="1">
-        <v>45077</v>
+        <v>45011</v>
       </c>
       <c r="E4" s="1">
-        <v>45133</v>
+        <v>45028</v>
       </c>
     </row>
     <row r="5" spans="1:6" x14ac:dyDescent="0.25">
@@ -632,10 +644,10 @@
         <v>7</v>
       </c>
       <c r="D5" s="1">
-        <v>45176</v>
+        <v>45077</v>
       </c>
       <c r="E5" s="1">
-        <v>45224</v>
+        <v>45133</v>
       </c>
     </row>
     <row r="6" spans="1:6" x14ac:dyDescent="0.25">
@@ -643,629 +655,1236 @@
         <v>5</v>
       </c>
       <c r="B6" t="s">
-        <v>12</v>
+        <v>4</v>
       </c>
       <c r="C6" t="s">
-        <v>11</v>
+        <v>7</v>
       </c>
       <c r="D6" s="1">
-        <v>44877</v>
+        <v>45176</v>
       </c>
       <c r="E6" s="1">
-        <v>44966</v>
-      </c>
-      <c r="F6" t="s">
-        <v>32</v>
+        <v>45224</v>
       </c>
     </row>
     <row r="7" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A7" t="s">
-        <v>21</v>
+        <v>5</v>
       </c>
       <c r="B7" t="s">
-        <v>12</v>
+        <v>11</v>
       </c>
       <c r="C7" t="s">
-        <v>11</v>
+        <v>42</v>
       </c>
       <c r="D7" s="1">
-        <v>44652</v>
+        <v>44877</v>
       </c>
       <c r="E7" s="1">
-        <v>44985</v>
+        <v>44966</v>
+      </c>
+      <c r="F7" t="s">
+        <v>31</v>
       </c>
     </row>
     <row r="8" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A8" t="s">
-        <v>19</v>
+        <v>5</v>
       </c>
       <c r="B8" t="s">
-        <v>20</v>
+        <v>11</v>
       </c>
       <c r="C8" t="s">
-        <v>7</v>
+        <v>43</v>
       </c>
       <c r="D8" s="1">
-        <v>45141</v>
+        <v>44877</v>
       </c>
       <c r="E8" s="1">
-        <v>45156</v>
+        <v>44966</v>
+      </c>
+      <c r="F8" t="s">
+        <v>31</v>
       </c>
     </row>
     <row r="9" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A9" t="s">
-        <v>19</v>
+        <v>5</v>
       </c>
       <c r="B9" t="s">
-        <v>4</v>
+        <v>11</v>
       </c>
       <c r="C9" t="s">
-        <v>25</v>
+        <v>44</v>
       </c>
       <c r="D9" s="1">
-        <v>44816</v>
+        <v>44877</v>
       </c>
       <c r="E9" s="1">
-        <v>44819</v>
+        <v>44966</v>
+      </c>
+      <c r="F9" t="s">
+        <v>31</v>
       </c>
     </row>
     <row r="10" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A10" t="s">
-        <v>13</v>
+        <v>20</v>
       </c>
       <c r="B10" t="s">
-        <v>22</v>
+        <v>11</v>
       </c>
       <c r="C10" t="s">
-        <v>11</v>
+        <v>42</v>
       </c>
       <c r="D10" s="1">
-        <v>45253</v>
+        <v>44652</v>
       </c>
       <c r="E10" s="1">
-        <v>45253</v>
+        <v>44985</v>
       </c>
     </row>
     <row r="11" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A11" t="s">
-        <v>13</v>
+        <v>20</v>
       </c>
       <c r="B11" t="s">
-        <v>12</v>
+        <v>11</v>
       </c>
       <c r="C11" t="s">
-        <v>11</v>
+        <v>43</v>
       </c>
       <c r="D11" s="1">
-        <v>44939</v>
+        <v>44652</v>
       </c>
       <c r="E11" s="1">
-        <v>44940</v>
+        <v>44985</v>
       </c>
     </row>
     <row r="12" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A12" t="s">
-        <v>13</v>
+        <v>20</v>
       </c>
       <c r="B12" t="s">
-        <v>12</v>
+        <v>11</v>
       </c>
       <c r="C12" t="s">
-        <v>11</v>
+        <v>44</v>
       </c>
       <c r="D12" s="1">
-        <v>44954</v>
+        <v>44652</v>
       </c>
       <c r="E12" s="1">
-        <v>44958</v>
+        <v>44985</v>
       </c>
     </row>
     <row r="13" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A13" t="s">
-        <v>13</v>
+        <v>18</v>
       </c>
       <c r="B13" t="s">
-        <v>12</v>
+        <v>19</v>
       </c>
       <c r="C13" t="s">
-        <v>11</v>
+        <v>7</v>
       </c>
       <c r="D13" s="1">
-        <v>44966</v>
+        <v>45141</v>
       </c>
       <c r="E13" s="1">
-        <v>44967</v>
+        <v>45156</v>
       </c>
     </row>
     <row r="14" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A14" t="s">
-        <v>13</v>
+        <v>18</v>
       </c>
       <c r="B14" t="s">
-        <v>12</v>
+        <v>4</v>
       </c>
       <c r="C14" t="s">
-        <v>11</v>
+        <v>24</v>
       </c>
       <c r="D14" s="1">
-        <v>45226</v>
+        <v>44816</v>
       </c>
       <c r="E14" s="1">
-        <v>45255</v>
+        <v>44819</v>
       </c>
     </row>
     <row r="15" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A15" t="s">
-        <v>14</v>
+        <v>12</v>
       </c>
       <c r="B15" t="s">
-        <v>12</v>
+        <v>21</v>
       </c>
       <c r="C15" t="s">
-        <v>11</v>
+        <v>42</v>
       </c>
       <c r="D15" s="1">
-        <v>45101</v>
+        <v>45253</v>
       </c>
       <c r="E15" s="1">
-        <v>45165</v>
+        <v>45253</v>
       </c>
     </row>
     <row r="16" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A16" t="s">
-        <v>14</v>
+        <v>12</v>
       </c>
       <c r="B16" t="s">
-        <v>4</v>
+        <v>21</v>
       </c>
       <c r="C16" t="s">
-        <v>23</v>
+        <v>43</v>
       </c>
       <c r="D16" s="1">
-        <v>45144</v>
+        <v>45253</v>
       </c>
       <c r="E16" s="1">
-        <v>45164</v>
-      </c>
-    </row>
-    <row r="17" spans="1:6" x14ac:dyDescent="0.25">
+        <v>45253</v>
+      </c>
+    </row>
+    <row r="17" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A17" t="s">
-        <v>10</v>
+        <v>12</v>
       </c>
       <c r="B17" t="s">
-        <v>4</v>
+        <v>21</v>
       </c>
       <c r="C17" t="s">
-        <v>11</v>
+        <v>44</v>
       </c>
       <c r="D17" s="1">
-        <v>44652</v>
+        <v>45253</v>
       </c>
       <c r="E17" s="1">
-        <v>44930</v>
-      </c>
-    </row>
-    <row r="18" spans="1:6" x14ac:dyDescent="0.25">
+        <v>45253</v>
+      </c>
+    </row>
+    <row r="18" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A18" t="s">
-        <v>40</v>
+        <v>12</v>
       </c>
       <c r="B18" t="s">
-        <v>4</v>
+        <v>11</v>
       </c>
       <c r="C18" t="s">
-        <v>7</v>
+        <v>42</v>
       </c>
       <c r="D18" s="1">
+        <v>44939</v>
+      </c>
+      <c r="E18" s="1">
+        <v>44940</v>
+      </c>
+    </row>
+    <row r="19" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A19" t="s">
+        <v>12</v>
+      </c>
+      <c r="B19" t="s">
+        <v>11</v>
+      </c>
+      <c r="C19" t="s">
+        <v>43</v>
+      </c>
+      <c r="D19" s="1">
+        <v>44939</v>
+      </c>
+      <c r="E19" s="1">
+        <v>44940</v>
+      </c>
+    </row>
+    <row r="20" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A20" t="s">
+        <v>12</v>
+      </c>
+      <c r="B20" t="s">
+        <v>11</v>
+      </c>
+      <c r="C20" t="s">
+        <v>44</v>
+      </c>
+      <c r="D20" s="1">
+        <v>44939</v>
+      </c>
+      <c r="E20" s="1">
+        <v>44940</v>
+      </c>
+    </row>
+    <row r="21" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A21" t="s">
+        <v>12</v>
+      </c>
+      <c r="B21" t="s">
+        <v>11</v>
+      </c>
+      <c r="C21" t="s">
+        <v>42</v>
+      </c>
+      <c r="D21" s="1">
+        <v>44954</v>
+      </c>
+      <c r="E21" s="1">
+        <v>44958</v>
+      </c>
+    </row>
+    <row r="22" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A22" t="s">
+        <v>12</v>
+      </c>
+      <c r="B22" t="s">
+        <v>11</v>
+      </c>
+      <c r="C22" t="s">
+        <v>43</v>
+      </c>
+      <c r="D22" s="1">
+        <v>44954</v>
+      </c>
+      <c r="E22" s="1">
+        <v>44958</v>
+      </c>
+    </row>
+    <row r="23" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A23" t="s">
+        <v>12</v>
+      </c>
+      <c r="B23" t="s">
+        <v>11</v>
+      </c>
+      <c r="C23" t="s">
+        <v>44</v>
+      </c>
+      <c r="D23" s="1">
+        <v>44954</v>
+      </c>
+      <c r="E23" s="1">
+        <v>44958</v>
+      </c>
+    </row>
+    <row r="24" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A24" t="s">
+        <v>12</v>
+      </c>
+      <c r="B24" t="s">
+        <v>11</v>
+      </c>
+      <c r="C24" t="s">
+        <v>42</v>
+      </c>
+      <c r="D24" s="1">
+        <v>44966</v>
+      </c>
+      <c r="E24" s="1">
         <v>44967</v>
       </c>
-      <c r="E18" s="1">
-        <v>45056</v>
-      </c>
-    </row>
-    <row r="19" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A19" t="s">
-        <v>16</v>
-      </c>
-      <c r="B19" t="s">
+    </row>
+    <row r="25" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A25" t="s">
         <v>12</v>
       </c>
-      <c r="C19" t="s">
-        <v>25</v>
-      </c>
-      <c r="D19" s="1">
-        <v>44652</v>
-      </c>
-      <c r="E19" s="1">
-        <v>44974</v>
-      </c>
-    </row>
-    <row r="20" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A20" t="s">
-        <v>16</v>
-      </c>
-      <c r="B20" t="s">
+      <c r="B25" t="s">
+        <v>11</v>
+      </c>
+      <c r="C25" t="s">
+        <v>43</v>
+      </c>
+      <c r="D25" s="1">
+        <v>44966</v>
+      </c>
+      <c r="E25" s="1">
+        <v>44967</v>
+      </c>
+    </row>
+    <row r="26" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A26" t="s">
         <v>12</v>
       </c>
-      <c r="C20" t="s">
-        <v>24</v>
-      </c>
-      <c r="D20" s="1">
-        <v>44652</v>
-      </c>
-      <c r="E20" s="1">
-        <v>44974</v>
-      </c>
-    </row>
-    <row r="21" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A21" t="s">
-        <v>16</v>
-      </c>
-      <c r="B21" t="s">
-        <v>12</v>
-      </c>
-      <c r="C21" t="s">
-        <v>11</v>
-      </c>
-      <c r="D21" s="1">
-        <v>44652</v>
-      </c>
-      <c r="E21" s="1">
-        <v>44974</v>
-      </c>
-    </row>
-    <row r="22" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A22" t="s">
-        <v>15</v>
-      </c>
-      <c r="B22" t="s">
-        <v>4</v>
-      </c>
-      <c r="C22" t="s">
-        <v>7</v>
-      </c>
-      <c r="D22" s="1">
-        <v>45140</v>
-      </c>
-      <c r="E22" s="1">
-        <v>45141</v>
-      </c>
-    </row>
-    <row r="23" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A23" t="s">
-        <v>15</v>
-      </c>
-      <c r="B23" t="s">
-        <v>22</v>
-      </c>
-      <c r="C23" t="s">
-        <v>24</v>
-      </c>
-      <c r="D23" s="1">
-        <v>44652</v>
-      </c>
-      <c r="E23" s="1">
-        <v>45027</v>
-      </c>
-      <c r="F23" t="s">
-        <v>27</v>
-      </c>
-    </row>
-    <row r="24" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A24" t="s">
-        <v>15</v>
-      </c>
-      <c r="B24" t="s">
-        <v>22</v>
-      </c>
-      <c r="C24" t="s">
-        <v>25</v>
-      </c>
-      <c r="D24" s="1">
-        <v>44652</v>
-      </c>
-      <c r="E24" s="1">
-        <v>45027</v>
-      </c>
-      <c r="F24" t="s">
-        <v>27</v>
-      </c>
-    </row>
-    <row r="25" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A25" t="s">
-        <v>15</v>
-      </c>
-      <c r="B25" t="s">
-        <v>12</v>
-      </c>
-      <c r="C25" t="s">
-        <v>11</v>
-      </c>
-      <c r="D25" s="1">
-        <v>44974</v>
-      </c>
-      <c r="E25" s="1">
-        <v>44986</v>
-      </c>
-    </row>
-    <row r="26" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A26" t="s">
-        <v>8</v>
-      </c>
       <c r="B26" t="s">
-        <v>4</v>
+        <v>11</v>
       </c>
       <c r="C26" t="s">
-        <v>9</v>
+        <v>44</v>
       </c>
       <c r="D26" s="1">
         <v>44966</v>
       </c>
       <c r="E26" s="1">
-        <v>45035</v>
-      </c>
-    </row>
-    <row r="27" spans="1:6" x14ac:dyDescent="0.25">
+        <v>44967</v>
+      </c>
+    </row>
+    <row r="27" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A27" t="s">
-        <v>8</v>
+        <v>12</v>
       </c>
       <c r="B27" t="s">
-        <v>20</v>
+        <v>11</v>
       </c>
       <c r="C27" t="s">
-        <v>7</v>
+        <v>42</v>
       </c>
       <c r="D27" s="1">
-        <v>45097</v>
+        <v>45226</v>
       </c>
       <c r="E27" s="1">
-        <v>45154</v>
-      </c>
-      <c r="F27" t="s">
-        <v>28</v>
-      </c>
-    </row>
-    <row r="28" spans="1:6" x14ac:dyDescent="0.25">
+        <v>45255</v>
+      </c>
+    </row>
+    <row r="28" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A28" t="s">
-        <v>8</v>
+        <v>12</v>
       </c>
       <c r="B28" t="s">
+        <v>11</v>
+      </c>
+      <c r="C28" t="s">
+        <v>43</v>
+      </c>
+      <c r="D28" s="1">
+        <v>45226</v>
+      </c>
+      <c r="E28" s="1">
+        <v>45255</v>
+      </c>
+    </row>
+    <row r="29" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A29" t="s">
         <v>12</v>
       </c>
-      <c r="C28" t="s">
-        <v>11</v>
-      </c>
-      <c r="D28" s="1">
-        <v>44953</v>
-      </c>
-      <c r="E28" s="1">
-        <v>46022</v>
-      </c>
-    </row>
-    <row r="29" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A29" t="s">
-        <v>29</v>
-      </c>
       <c r="B29" t="s">
-        <v>22</v>
+        <v>11</v>
       </c>
       <c r="C29" t="s">
-        <v>7</v>
+        <v>44</v>
       </c>
       <c r="D29" s="1">
-        <v>45113</v>
+        <v>45226</v>
       </c>
       <c r="E29" s="1">
-        <v>45140</v>
-      </c>
-    </row>
-    <row r="30" spans="1:6" x14ac:dyDescent="0.25">
+        <v>45255</v>
+      </c>
+    </row>
+    <row r="30" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A30" t="s">
-        <v>29</v>
+        <v>13</v>
       </c>
       <c r="B30" t="s">
-        <v>22</v>
+        <v>11</v>
       </c>
       <c r="C30" t="s">
-        <v>7</v>
+        <v>42</v>
       </c>
       <c r="D30" s="1">
-        <v>45176</v>
+        <v>45101</v>
       </c>
       <c r="E30" s="1">
-        <v>45190</v>
-      </c>
-    </row>
-    <row r="31" spans="1:6" x14ac:dyDescent="0.25">
+        <v>45165</v>
+      </c>
+    </row>
+    <row r="31" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A31" t="s">
-        <v>29</v>
+        <v>13</v>
       </c>
       <c r="B31" t="s">
-        <v>22</v>
+        <v>11</v>
       </c>
       <c r="C31" t="s">
-        <v>7</v>
+        <v>43</v>
       </c>
       <c r="D31" s="1">
-        <v>45258</v>
+        <v>45101</v>
       </c>
       <c r="E31" s="1">
-        <v>45268</v>
-      </c>
-    </row>
-    <row r="32" spans="1:6" x14ac:dyDescent="0.25">
+        <v>45165</v>
+      </c>
+    </row>
+    <row r="32" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A32" t="s">
-        <v>29</v>
+        <v>13</v>
       </c>
       <c r="B32" t="s">
-        <v>4</v>
+        <v>11</v>
       </c>
       <c r="C32" t="s">
-        <v>23</v>
+        <v>44</v>
       </c>
       <c r="D32" s="1">
-        <v>45222</v>
+        <v>45101</v>
       </c>
       <c r="E32" s="1">
-        <v>45398</v>
+        <v>45165</v>
       </c>
     </row>
     <row r="33" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A33" t="s">
-        <v>18</v>
+        <v>13</v>
       </c>
       <c r="B33" t="s">
+        <v>4</v>
+      </c>
+      <c r="C33" t="s">
         <v>22</v>
       </c>
-      <c r="C33" t="s">
-        <v>7</v>
-      </c>
       <c r="D33" s="1">
-        <v>45222</v>
+        <v>45144</v>
       </c>
       <c r="E33" s="1">
-        <v>45237</v>
+        <v>45164</v>
       </c>
     </row>
     <row r="34" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A34" t="s">
-        <v>18</v>
+        <v>10</v>
       </c>
       <c r="B34" t="s">
-        <v>12</v>
+        <v>4</v>
       </c>
       <c r="C34" t="s">
-        <v>11</v>
+        <v>42</v>
       </c>
       <c r="D34" s="1">
-        <v>45252</v>
+        <v>44652</v>
       </c>
       <c r="E34" s="1">
-        <v>45351</v>
+        <v>44930</v>
       </c>
     </row>
     <row r="35" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A35" t="s">
-        <v>17</v>
+        <v>10</v>
       </c>
       <c r="B35" t="s">
-        <v>30</v>
+        <v>4</v>
       </c>
       <c r="C35" t="s">
-        <v>7</v>
+        <v>43</v>
       </c>
       <c r="D35" s="1">
-        <v>45101</v>
+        <v>44652</v>
       </c>
       <c r="E35" s="1">
-        <v>45133</v>
+        <v>44930</v>
       </c>
     </row>
     <row r="36" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A36" t="s">
-        <v>17</v>
+        <v>10</v>
       </c>
       <c r="B36" t="s">
-        <v>30</v>
+        <v>4</v>
       </c>
       <c r="C36" t="s">
-        <v>7</v>
+        <v>44</v>
       </c>
       <c r="D36" s="1">
-        <v>45153</v>
+        <v>44652</v>
       </c>
       <c r="E36" s="1">
-        <v>45188</v>
+        <v>44930</v>
       </c>
     </row>
     <row r="37" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A37" t="s">
-        <v>17</v>
+        <v>39</v>
       </c>
       <c r="B37" t="s">
-        <v>12</v>
+        <v>4</v>
       </c>
       <c r="C37" t="s">
-        <v>11</v>
+        <v>7</v>
       </c>
       <c r="D37" s="1">
-        <v>45076</v>
+        <v>44967</v>
       </c>
       <c r="E37" s="1">
-        <v>45351</v>
+        <v>45056</v>
       </c>
     </row>
     <row r="38" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A38" t="s">
-        <v>31</v>
+        <v>15</v>
       </c>
       <c r="B38" t="s">
-        <v>30</v>
+        <v>11</v>
       </c>
       <c r="C38" t="s">
-        <v>7</v>
+        <v>24</v>
       </c>
       <c r="D38" s="1">
-        <v>44882</v>
+        <v>44652</v>
       </c>
       <c r="E38" s="1">
-        <v>44931</v>
+        <v>44974</v>
       </c>
     </row>
     <row r="39" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A39" t="s">
-        <v>35</v>
+        <v>15</v>
       </c>
       <c r="B39" t="s">
-        <v>22</v>
+        <v>11</v>
       </c>
       <c r="C39" t="s">
-        <v>7</v>
+        <v>23</v>
       </c>
       <c r="D39" s="1">
-        <v>45282</v>
+        <v>44652</v>
       </c>
       <c r="E39" s="1">
-        <v>45401</v>
+        <v>44974</v>
       </c>
     </row>
     <row r="40" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A40" t="s">
-        <v>35</v>
+        <v>15</v>
       </c>
       <c r="B40" t="s">
-        <v>4</v>
+        <v>11</v>
       </c>
       <c r="C40" t="s">
-        <v>23</v>
+        <v>42</v>
       </c>
       <c r="D40" s="1">
-        <v>44856</v>
+        <v>44652</v>
       </c>
       <c r="E40" s="1">
-        <v>44883</v>
-      </c>
-      <c r="F40" t="s">
-        <v>36</v>
+        <v>44974</v>
       </c>
     </row>
     <row r="41" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A41" t="s">
+        <v>15</v>
+      </c>
+      <c r="B41" t="s">
+        <v>11</v>
+      </c>
+      <c r="C41" t="s">
+        <v>43</v>
+      </c>
+      <c r="D41" s="1">
+        <v>44652</v>
+      </c>
+      <c r="E41" s="1">
+        <v>44974</v>
+      </c>
+    </row>
+    <row r="42" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A42" t="s">
+        <v>15</v>
+      </c>
+      <c r="B42" t="s">
+        <v>11</v>
+      </c>
+      <c r="C42" t="s">
+        <v>44</v>
+      </c>
+      <c r="D42" s="1">
+        <v>44652</v>
+      </c>
+      <c r="E42" s="1">
+        <v>44974</v>
+      </c>
+    </row>
+    <row r="43" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A43" t="s">
+        <v>14</v>
+      </c>
+      <c r="B43" t="s">
+        <v>4</v>
+      </c>
+      <c r="C43" t="s">
+        <v>7</v>
+      </c>
+      <c r="D43" s="1">
+        <v>45140</v>
+      </c>
+      <c r="E43" s="1">
+        <v>45141</v>
+      </c>
+    </row>
+    <row r="44" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A44" t="s">
+        <v>14</v>
+      </c>
+      <c r="B44" t="s">
+        <v>21</v>
+      </c>
+      <c r="C44" t="s">
+        <v>23</v>
+      </c>
+      <c r="D44" s="1">
+        <v>44652</v>
+      </c>
+      <c r="E44" s="1">
+        <v>45027</v>
+      </c>
+      <c r="F44" t="s">
+        <v>26</v>
+      </c>
+    </row>
+    <row r="45" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A45" t="s">
+        <v>14</v>
+      </c>
+      <c r="B45" t="s">
+        <v>21</v>
+      </c>
+      <c r="C45" t="s">
+        <v>24</v>
+      </c>
+      <c r="D45" s="1">
+        <v>44652</v>
+      </c>
+      <c r="E45" s="1">
+        <v>45027</v>
+      </c>
+      <c r="F45" t="s">
+        <v>26</v>
+      </c>
+    </row>
+    <row r="46" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A46" t="s">
+        <v>14</v>
+      </c>
+      <c r="B46" t="s">
+        <v>11</v>
+      </c>
+      <c r="C46" t="s">
+        <v>42</v>
+      </c>
+      <c r="D46" s="1">
+        <v>44974</v>
+      </c>
+      <c r="E46" s="1">
+        <v>44986</v>
+      </c>
+    </row>
+    <row r="47" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A47" t="s">
+        <v>14</v>
+      </c>
+      <c r="B47" t="s">
+        <v>11</v>
+      </c>
+      <c r="C47" t="s">
+        <v>43</v>
+      </c>
+      <c r="D47" s="1">
+        <v>44974</v>
+      </c>
+      <c r="E47" s="1">
+        <v>44986</v>
+      </c>
+    </row>
+    <row r="48" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A48" t="s">
+        <v>14</v>
+      </c>
+      <c r="B48" t="s">
+        <v>11</v>
+      </c>
+      <c r="C48" t="s">
+        <v>44</v>
+      </c>
+      <c r="D48" s="1">
+        <v>44974</v>
+      </c>
+      <c r="E48" s="1">
+        <v>44986</v>
+      </c>
+    </row>
+    <row r="49" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A49" t="s">
+        <v>8</v>
+      </c>
+      <c r="B49" t="s">
+        <v>4</v>
+      </c>
+      <c r="C49" t="s">
+        <v>9</v>
+      </c>
+      <c r="D49" s="1">
+        <v>44966</v>
+      </c>
+      <c r="E49" s="1">
+        <v>45035</v>
+      </c>
+    </row>
+    <row r="50" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A50" t="s">
+        <v>8</v>
+      </c>
+      <c r="B50" t="s">
+        <v>19</v>
+      </c>
+      <c r="C50" t="s">
+        <v>7</v>
+      </c>
+      <c r="D50" s="1">
+        <v>45097</v>
+      </c>
+      <c r="E50" s="1">
+        <v>45154</v>
+      </c>
+      <c r="F50" t="s">
+        <v>27</v>
+      </c>
+    </row>
+    <row r="51" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A51" t="s">
+        <v>8</v>
+      </c>
+      <c r="B51" t="s">
+        <v>11</v>
+      </c>
+      <c r="C51" t="s">
+        <v>42</v>
+      </c>
+      <c r="D51" s="1">
+        <v>44953</v>
+      </c>
+      <c r="E51" s="1">
+        <v>46022</v>
+      </c>
+    </row>
+    <row r="52" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A52" t="s">
+        <v>8</v>
+      </c>
+      <c r="B52" t="s">
+        <v>11</v>
+      </c>
+      <c r="C52" t="s">
+        <v>43</v>
+      </c>
+      <c r="D52" s="1">
+        <v>44953</v>
+      </c>
+      <c r="E52" s="1">
+        <v>46022</v>
+      </c>
+    </row>
+    <row r="53" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A53" t="s">
+        <v>8</v>
+      </c>
+      <c r="B53" t="s">
+        <v>11</v>
+      </c>
+      <c r="C53" t="s">
+        <v>44</v>
+      </c>
+      <c r="D53" s="1">
+        <v>44953</v>
+      </c>
+      <c r="E53" s="1">
+        <v>46022</v>
+      </c>
+    </row>
+    <row r="54" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A54" t="s">
+        <v>28</v>
+      </c>
+      <c r="B54" t="s">
+        <v>29</v>
+      </c>
+      <c r="C54" t="s">
+        <v>7</v>
+      </c>
+      <c r="D54" s="1">
+        <v>45185</v>
+      </c>
+      <c r="E54" s="1">
+        <v>45190</v>
+      </c>
+    </row>
+    <row r="55" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A55" t="s">
+        <v>28</v>
+      </c>
+      <c r="B55" t="s">
+        <v>21</v>
+      </c>
+      <c r="C55" t="s">
+        <v>7</v>
+      </c>
+      <c r="D55" s="1">
+        <v>45113</v>
+      </c>
+      <c r="E55" s="1">
+        <v>45140</v>
+      </c>
+    </row>
+    <row r="56" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A56" t="s">
+        <v>28</v>
+      </c>
+      <c r="B56" t="s">
+        <v>21</v>
+      </c>
+      <c r="C56" t="s">
+        <v>7</v>
+      </c>
+      <c r="D56" s="1">
+        <v>45176</v>
+      </c>
+      <c r="E56" s="1">
+        <v>45190</v>
+      </c>
+    </row>
+    <row r="57" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A57" t="s">
+        <v>28</v>
+      </c>
+      <c r="B57" t="s">
+        <v>21</v>
+      </c>
+      <c r="C57" t="s">
+        <v>7</v>
+      </c>
+      <c r="D57" s="1">
+        <v>45258</v>
+      </c>
+      <c r="E57" s="1">
+        <v>45268</v>
+      </c>
+    </row>
+    <row r="58" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A58" t="s">
+        <v>28</v>
+      </c>
+      <c r="B58" t="s">
+        <v>4</v>
+      </c>
+      <c r="C58" t="s">
+        <v>22</v>
+      </c>
+      <c r="D58" s="1">
+        <v>45222</v>
+      </c>
+      <c r="E58" s="1">
+        <v>45398</v>
+      </c>
+    </row>
+    <row r="59" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A59" t="s">
+        <v>17</v>
+      </c>
+      <c r="B59" t="s">
+        <v>21</v>
+      </c>
+      <c r="C59" t="s">
+        <v>7</v>
+      </c>
+      <c r="D59" s="1">
+        <v>45222</v>
+      </c>
+      <c r="E59" s="1">
+        <v>45237</v>
+      </c>
+    </row>
+    <row r="60" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A60" t="s">
+        <v>17</v>
+      </c>
+      <c r="B60" t="s">
+        <v>11</v>
+      </c>
+      <c r="C60" t="s">
+        <v>42</v>
+      </c>
+      <c r="D60" s="1">
+        <v>45252</v>
+      </c>
+      <c r="E60" s="1">
+        <v>45351</v>
+      </c>
+    </row>
+    <row r="61" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A61" t="s">
+        <v>17</v>
+      </c>
+      <c r="B61" t="s">
+        <v>11</v>
+      </c>
+      <c r="C61" t="s">
+        <v>43</v>
+      </c>
+      <c r="D61" s="1">
+        <v>45252</v>
+      </c>
+      <c r="E61" s="1">
+        <v>45351</v>
+      </c>
+    </row>
+    <row r="62" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A62" t="s">
+        <v>17</v>
+      </c>
+      <c r="B62" t="s">
+        <v>11</v>
+      </c>
+      <c r="C62" t="s">
+        <v>44</v>
+      </c>
+      <c r="D62" s="1">
+        <v>45252</v>
+      </c>
+      <c r="E62" s="1">
+        <v>45351</v>
+      </c>
+    </row>
+    <row r="63" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A63" t="s">
+        <v>16</v>
+      </c>
+      <c r="B63" t="s">
+        <v>29</v>
+      </c>
+      <c r="C63" t="s">
+        <v>7</v>
+      </c>
+      <c r="D63" s="1">
+        <v>45101</v>
+      </c>
+      <c r="E63" s="1">
+        <v>45133</v>
+      </c>
+    </row>
+    <row r="64" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A64" t="s">
+        <v>16</v>
+      </c>
+      <c r="B64" t="s">
+        <v>29</v>
+      </c>
+      <c r="C64" t="s">
+        <v>7</v>
+      </c>
+      <c r="D64" s="1">
+        <v>45153</v>
+      </c>
+      <c r="E64" s="1">
+        <v>45188</v>
+      </c>
+    </row>
+    <row r="65" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A65" t="s">
+        <v>16</v>
+      </c>
+      <c r="B65" t="s">
+        <v>11</v>
+      </c>
+      <c r="C65" t="s">
+        <v>42</v>
+      </c>
+      <c r="D65" s="1">
+        <v>45076</v>
+      </c>
+      <c r="E65" s="1">
+        <v>45351</v>
+      </c>
+    </row>
+    <row r="66" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A66" t="s">
+        <v>16</v>
+      </c>
+      <c r="B66" t="s">
+        <v>11</v>
+      </c>
+      <c r="C66" t="s">
+        <v>43</v>
+      </c>
+      <c r="D66" s="1">
+        <v>45076</v>
+      </c>
+      <c r="E66" s="1">
+        <v>45351</v>
+      </c>
+    </row>
+    <row r="67" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A67" t="s">
+        <v>16</v>
+      </c>
+      <c r="B67" t="s">
+        <v>11</v>
+      </c>
+      <c r="C67" t="s">
+        <v>44</v>
+      </c>
+      <c r="D67" s="1">
+        <v>45076</v>
+      </c>
+      <c r="E67" s="1">
+        <v>45351</v>
+      </c>
+    </row>
+    <row r="68" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A68" t="s">
+        <v>30</v>
+      </c>
+      <c r="B68" t="s">
+        <v>29</v>
+      </c>
+      <c r="C68" t="s">
+        <v>7</v>
+      </c>
+      <c r="D68" s="1">
+        <v>44882</v>
+      </c>
+      <c r="E68" s="1">
+        <v>44931</v>
+      </c>
+    </row>
+    <row r="69" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A69" t="s">
+        <v>30</v>
+      </c>
+      <c r="B69" t="s">
+        <v>29</v>
+      </c>
+      <c r="C69" t="s">
+        <v>7</v>
+      </c>
+      <c r="D69" s="1">
+        <v>44932</v>
+      </c>
+      <c r="E69" s="1">
+        <v>44941</v>
+      </c>
+      <c r="F69" t="s">
+        <v>40</v>
+      </c>
+    </row>
+    <row r="70" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A70" t="s">
+        <v>34</v>
+      </c>
+      <c r="B70" t="s">
+        <v>19</v>
+      </c>
+      <c r="C70" t="s">
+        <v>7</v>
+      </c>
+      <c r="D70" s="1">
+        <v>44652</v>
+      </c>
+      <c r="E70" s="1">
+        <v>44783</v>
+      </c>
+    </row>
+    <row r="71" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A71" t="s">
+        <v>34</v>
+      </c>
+      <c r="B71" t="s">
+        <v>21</v>
+      </c>
+      <c r="C71" t="s">
+        <v>7</v>
+      </c>
+      <c r="D71" s="1">
+        <v>45282</v>
+      </c>
+      <c r="E71" s="1">
+        <v>45401</v>
+      </c>
+    </row>
+    <row r="72" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A72" t="s">
+        <v>34</v>
+      </c>
+      <c r="B72" t="s">
+        <v>4</v>
+      </c>
+      <c r="C72" t="s">
+        <v>22</v>
+      </c>
+      <c r="D72" s="1">
+        <v>44856</v>
+      </c>
+      <c r="E72" s="1">
+        <v>44883</v>
+      </c>
+      <c r="F72" t="s">
+        <v>35</v>
+      </c>
+    </row>
+    <row r="73" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A73" t="s">
+        <v>36</v>
+      </c>
+      <c r="B73" t="s">
         <v>37</v>
       </c>
-      <c r="B41" t="s">
+      <c r="C73" t="s">
+        <v>24</v>
+      </c>
+      <c r="D73" s="1">
+        <v>45194</v>
+      </c>
+      <c r="E73" s="1">
+        <v>45244</v>
+      </c>
+      <c r="F73" t="s">
         <v>38</v>
       </c>
-      <c r="C41" t="s">
-        <v>25</v>
-      </c>
-      <c r="D41" s="1">
+    </row>
+    <row r="74" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A74" t="s">
+        <v>36</v>
+      </c>
+      <c r="B74" t="s">
+        <v>37</v>
+      </c>
+      <c r="C74" t="s">
+        <v>42</v>
+      </c>
+      <c r="D74" s="1">
         <v>45194</v>
       </c>
-      <c r="E41" s="1">
+      <c r="E74" s="1">
         <v>45244</v>
       </c>
-      <c r="F41" t="s">
-        <v>39</v>
+      <c r="F74" t="s">
+        <v>41</v>
+      </c>
+    </row>
+    <row r="75" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A75" t="s">
+        <v>36</v>
+      </c>
+      <c r="B75" t="s">
+        <v>37</v>
+      </c>
+      <c r="C75" t="s">
+        <v>43</v>
+      </c>
+      <c r="D75" s="1">
+        <v>45194</v>
+      </c>
+      <c r="E75" s="1">
+        <v>45244</v>
+      </c>
+    </row>
+    <row r="76" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A76" t="s">
+        <v>36</v>
+      </c>
+      <c r="B76" t="s">
+        <v>37</v>
+      </c>
+      <c r="C76" t="s">
+        <v>44</v>
+      </c>
+      <c r="D76" s="1">
+        <v>45194</v>
+      </c>
+      <c r="E76" s="1">
+        <v>45244</v>
       </c>
     </row>
   </sheetData>

</xml_diff>